<commit_message>
Group project 1 stuff
</commit_message>
<xml_diff>
--- a/projects/P1 -  Excel Grading/Well_Organized_Data_1.xlsx
+++ b/projects/P1 -  Excel Grading/Well_Organized_Data_1.xlsx
@@ -7,7 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Algebra" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Trigonometry" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Geometry" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Calculus" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Statistics" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +21,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +53,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +421,466 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Summary Statistics</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Highest Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Lowest Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mean Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Median Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Number of Students</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Summary Statistics</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Highest Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Lowest Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mean Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Median Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Number of Students</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Summary Statistics</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Highest Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Lowest Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mean Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Median Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Number of Students</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Summary Statistics</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Highest Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Lowest Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mean Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Median Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Number of Students</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Summary Statistics</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Highest Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Lowest Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mean Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Median Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Number of Students</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Functions for max, min, avg, med, and count
</commit_message>
<xml_diff>
--- a/projects/P1 -  Excel Grading/Well_Organized_Data_1.xlsx
+++ b/projects/P1 -  Excel Grading/Well_Organized_Data_1.xlsx
@@ -475,6 +475,10 @@
           <t>Highest Grade</t>
         </is>
       </c>
+      <c r="G2">
+        <f>MAX(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="F3" t="inlineStr">
@@ -482,6 +486,10 @@
           <t>Lowest Grade</t>
         </is>
       </c>
+      <c r="G3">
+        <f>MIN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="F4" t="inlineStr">
@@ -489,6 +497,10 @@
           <t>Mean Grade</t>
         </is>
       </c>
+      <c r="G4">
+        <f>IF(G6=0,0,AVERAGE(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="F5" t="inlineStr">
@@ -496,12 +508,20 @@
           <t>Median Grade</t>
         </is>
       </c>
+      <c r="G5">
+        <f>IF(G6=0,0,MEDIAN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="F6" t="inlineStr">
         <is>
           <t>Number of Students</t>
         </is>
+      </c>
+      <c r="G6">
+        <f>COUNT(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -569,6 +589,10 @@
           <t>Highest Grade</t>
         </is>
       </c>
+      <c r="G2">
+        <f>MAX(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="F3" t="inlineStr">
@@ -576,6 +600,10 @@
           <t>Lowest Grade</t>
         </is>
       </c>
+      <c r="G3">
+        <f>MIN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="F4" t="inlineStr">
@@ -583,6 +611,10 @@
           <t>Mean Grade</t>
         </is>
       </c>
+      <c r="G4">
+        <f>IF(G6=0,0,AVERAGE(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="F5" t="inlineStr">
@@ -590,12 +622,20 @@
           <t>Median Grade</t>
         </is>
       </c>
+      <c r="G5">
+        <f>IF(G6=0,0,MEDIAN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="F6" t="inlineStr">
         <is>
           <t>Number of Students</t>
         </is>
+      </c>
+      <c r="G6">
+        <f>COUNT(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -663,6 +703,10 @@
           <t>Highest Grade</t>
         </is>
       </c>
+      <c r="G2">
+        <f>MAX(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="F3" t="inlineStr">
@@ -670,6 +714,10 @@
           <t>Lowest Grade</t>
         </is>
       </c>
+      <c r="G3">
+        <f>MIN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="F4" t="inlineStr">
@@ -677,6 +725,10 @@
           <t>Mean Grade</t>
         </is>
       </c>
+      <c r="G4">
+        <f>IF(G6=0,0,AVERAGE(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="F5" t="inlineStr">
@@ -684,12 +736,20 @@
           <t>Median Grade</t>
         </is>
       </c>
+      <c r="G5">
+        <f>IF(G6=0,0,MEDIAN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="F6" t="inlineStr">
         <is>
           <t>Number of Students</t>
         </is>
+      </c>
+      <c r="G6">
+        <f>COUNT(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -757,6 +817,10 @@
           <t>Highest Grade</t>
         </is>
       </c>
+      <c r="G2">
+        <f>MAX(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="F3" t="inlineStr">
@@ -764,6 +828,10 @@
           <t>Lowest Grade</t>
         </is>
       </c>
+      <c r="G3">
+        <f>MIN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="F4" t="inlineStr">
@@ -771,6 +839,10 @@
           <t>Mean Grade</t>
         </is>
       </c>
+      <c r="G4">
+        <f>IF(G6=0,0,AVERAGE(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="F5" t="inlineStr">
@@ -778,12 +850,20 @@
           <t>Median Grade</t>
         </is>
       </c>
+      <c r="G5">
+        <f>IF(G6=0,0,MEDIAN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="F6" t="inlineStr">
         <is>
           <t>Number of Students</t>
         </is>
+      </c>
+      <c r="G6">
+        <f>COUNT(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -851,6 +931,10 @@
           <t>Highest Grade</t>
         </is>
       </c>
+      <c r="G2">
+        <f>MAX(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="F3" t="inlineStr">
@@ -858,6 +942,10 @@
           <t>Lowest Grade</t>
         </is>
       </c>
+      <c r="G3">
+        <f>MIN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="F4" t="inlineStr">
@@ -865,6 +953,10 @@
           <t>Mean Grade</t>
         </is>
       </c>
+      <c r="G4">
+        <f>IF(G6=0,0,AVERAGE(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="F5" t="inlineStr">
@@ -872,12 +964,20 @@
           <t>Median Grade</t>
         </is>
       </c>
+      <c r="G5">
+        <f>IF(G6=0,0,MEDIAN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="F6" t="inlineStr">
         <is>
           <t>Number of Students</t>
         </is>
+      </c>
+      <c r="G6">
+        <f>COUNT(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>